<commit_message>
IMDI: Added German Translations for Corpus Comments
</commit_message>
<xml_diff>
--- a/docs/CMDI Maker Localisations.xlsx
+++ b/docs/CMDI Maker Localisations.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Documents\GitHub\CMDI-Maker\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="588" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="585"/>
   </bookViews>
   <sheets>
     <sheet name="APP CORE" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="504">
   <si>
     <t>Key1</t>
   </si>
@@ -1531,6 +1531,12 @@
   </si>
   <si>
     <t>Corpus inklusive aller Sessions herunterladen</t>
+  </si>
+  <si>
+    <t>Ein kurzer, archivierbarer Name für dein Korpus.</t>
+  </si>
+  <si>
+    <t>Der komplette und ausführliche Titel deines Korpus.</t>
   </si>
 </sst>
 </file>
@@ -1540,7 +1546,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1901,25 +1907,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="4"/>
+    <col min="1" max="1" width="11.5" style="4"/>
     <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="4"/>
-    <col min="5" max="5" width="30.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.25" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="4"/>
+    <col min="5" max="5" width="30.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="32" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.5546875" style="2"/>
+    <col min="7" max="7" width="31.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1939,7 +1945,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1953,7 +1959,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1967,7 +1973,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1981,7 +1987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -1995,7 +2001,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2023,7 +2029,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -2037,7 +2043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -2051,7 +2057,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -2065,7 +2071,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -2079,7 +2085,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="57">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -2093,7 +2099,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -2107,7 +2113,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="57">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -2121,7 +2127,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -2135,7 +2141,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="28.5">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -2149,7 +2155,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -2163,7 +2169,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" ht="156.75">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -2177,7 +2183,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
@@ -2191,7 +2197,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="42.75">
       <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
@@ -2205,7 +2211,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -2219,7 +2225,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="28.5">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -2233,7 +2239,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
@@ -2247,7 +2253,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="28.5">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
@@ -2261,7 +2267,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6">
       <c r="A25" s="4" t="s">
         <v>50</v>
       </c>
@@ -2275,7 +2281,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
@@ -2303,7 +2309,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
@@ -2317,7 +2323,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="28.5">
       <c r="A29" s="4" t="s">
         <v>54</v>
       </c>
@@ -2331,7 +2337,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" ht="42.75">
       <c r="A30" s="4" t="s">
         <v>54</v>
       </c>
@@ -2345,7 +2351,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
         <v>65</v>
       </c>
@@ -2356,7 +2362,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
         <v>11</v>
       </c>
@@ -2367,7 +2373,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>66</v>
       </c>
@@ -2378,7 +2384,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6">
       <c r="A34" s="4" t="s">
         <v>69</v>
       </c>
@@ -2389,7 +2395,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -2400,7 +2406,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>72</v>
       </c>
@@ -2411,7 +2417,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="99.75">
       <c r="A37" s="4" t="s">
         <v>75</v>
       </c>
@@ -2425,7 +2431,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>75</v>
       </c>
@@ -2439,7 +2445,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>75</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6">
       <c r="A40" s="4" t="s">
         <v>75</v>
       </c>
@@ -2467,7 +2473,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="57">
       <c r="A41" s="4" t="s">
         <v>75</v>
       </c>
@@ -2481,7 +2487,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6">
       <c r="A42" s="4" t="s">
         <v>75</v>
       </c>
@@ -2495,7 +2501,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
         <v>75</v>
       </c>
@@ -2512,7 +2518,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
         <v>75</v>
       </c>
@@ -2539,25 +2545,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F121" sqref="F121"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="4"/>
+    <col min="1" max="1" width="11.5" style="4"/>
     <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="4"/>
-    <col min="5" max="5" width="30.5546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.25" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.5" style="4"/>
+    <col min="5" max="5" width="30.5" style="2" customWidth="1"/>
     <col min="6" max="6" width="32" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.5546875" style="2"/>
+    <col min="7" max="7" width="31.375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.5" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2577,7 +2583,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6">
       <c r="A2" s="4" t="s">
         <v>131</v>
       </c>
@@ -2591,7 +2597,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6">
       <c r="A3" s="4" t="s">
         <v>131</v>
       </c>
@@ -2605,7 +2611,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6">
       <c r="A4" s="4" t="s">
         <v>131</v>
       </c>
@@ -2619,7 +2625,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6">
       <c r="A5" s="4" t="s">
         <v>131</v>
       </c>
@@ -2633,7 +2639,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6">
       <c r="A6" s="4" t="s">
         <v>131</v>
       </c>
@@ -2647,7 +2653,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="28.5">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2661,7 +2667,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="156.75">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -2675,7 +2681,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -2689,7 +2695,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -2703,7 +2709,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -2717,7 +2723,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -2731,7 +2737,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="28.5">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -2745,7 +2751,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="28.5">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -2759,7 +2765,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -2773,7 +2779,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="71.25">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -2787,7 +2793,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6">
       <c r="A17" s="4" t="s">
         <v>147</v>
       </c>
@@ -2798,7 +2804,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6">
       <c r="A18" s="4" t="s">
         <v>148</v>
       </c>
@@ -2809,7 +2815,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6">
       <c r="A19" s="4" t="s">
         <v>55</v>
       </c>
@@ -2820,7 +2826,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="42.75">
       <c r="A20" s="4" t="s">
         <v>149</v>
       </c>
@@ -2831,7 +2837,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6">
       <c r="A21" s="4" t="s">
         <v>150</v>
       </c>
@@ -2842,7 +2848,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6">
       <c r="A22" s="4" t="s">
         <v>151</v>
       </c>
@@ -2853,7 +2859,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6">
       <c r="A23" s="4" t="s">
         <v>66</v>
       </c>
@@ -2864,7 +2870,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="28.5">
       <c r="A24" s="4" t="s">
         <v>152</v>
       </c>
@@ -2875,7 +2881,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="28.5">
       <c r="A25" s="4" t="s">
         <v>174</v>
       </c>
@@ -2889,7 +2895,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6">
       <c r="A26" s="4" t="s">
         <v>174</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6">
       <c r="A27" s="4" t="s">
         <v>174</v>
       </c>
@@ -2917,7 +2923,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6">
       <c r="A28" s="4" t="s">
         <v>174</v>
       </c>
@@ -2931,7 +2937,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6">
       <c r="A29" s="4" t="s">
         <v>174</v>
       </c>
@@ -2945,7 +2951,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6">
       <c r="A30" s="4" t="s">
         <v>174</v>
       </c>
@@ -2959,7 +2965,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6">
       <c r="A31" s="4" t="s">
         <v>174</v>
       </c>
@@ -2973,7 +2979,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6">
       <c r="A32" s="4" t="s">
         <v>174</v>
       </c>
@@ -2987,7 +2993,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6">
       <c r="A33" s="4" t="s">
         <v>174</v>
       </c>
@@ -3001,7 +3007,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="42.75">
       <c r="A34" s="4" t="s">
         <v>174</v>
       </c>
@@ -3015,7 +3021,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6">
       <c r="A35" s="4" t="s">
         <v>174</v>
       </c>
@@ -3029,7 +3035,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6">
       <c r="A36" s="4" t="s">
         <v>174</v>
       </c>
@@ -3043,7 +3049,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6">
       <c r="A37" s="4" t="s">
         <v>174</v>
       </c>
@@ -3057,7 +3063,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6">
       <c r="A38" s="4" t="s">
         <v>174</v>
       </c>
@@ -3071,7 +3077,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6">
       <c r="A39" s="4" t="s">
         <v>174</v>
       </c>
@@ -3085,7 +3091,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="42.75">
       <c r="A40" s="4" t="s">
         <v>133</v>
       </c>
@@ -3102,7 +3108,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="57">
       <c r="A41" s="4" t="s">
         <v>133</v>
       </c>
@@ -3119,7 +3125,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="57">
       <c r="A42" s="4" t="s">
         <v>133</v>
       </c>
@@ -3136,7 +3142,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6">
       <c r="A43" s="4" t="s">
         <v>133</v>
       </c>
@@ -3150,7 +3156,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6">
       <c r="A44" s="4" t="s">
         <v>133</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6">
       <c r="A45" s="4" t="s">
         <v>133</v>
       </c>
@@ -3178,7 +3184,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6">
       <c r="A46" s="4" t="s">
         <v>133</v>
       </c>
@@ -3192,7 +3198,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6">
       <c r="A47" s="4" t="s">
         <v>133</v>
       </c>
@@ -3206,7 +3212,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6">
       <c r="A48" s="4" t="s">
         <v>133</v>
       </c>
@@ -3220,7 +3226,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6">
       <c r="A49" s="4" t="s">
         <v>133</v>
       </c>
@@ -3234,7 +3240,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6">
       <c r="A50" s="4" t="s">
         <v>133</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6">
       <c r="A51" s="4" t="s">
         <v>133</v>
       </c>
@@ -3262,7 +3268,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6">
       <c r="A52" s="4" t="s">
         <v>133</v>
       </c>
@@ -3276,7 +3282,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" ht="28.5">
       <c r="A53" s="4" t="s">
         <v>133</v>
       </c>
@@ -3290,7 +3296,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6">
       <c r="A54" s="4" t="s">
         <v>133</v>
       </c>
@@ -3304,7 +3310,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" ht="28.5">
       <c r="A55" s="4" t="s">
         <v>133</v>
       </c>
@@ -3318,7 +3324,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6">
       <c r="A56" s="4" t="s">
         <v>133</v>
       </c>
@@ -3332,7 +3338,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" ht="28.5">
       <c r="A57" s="4" t="s">
         <v>133</v>
       </c>
@@ -3346,7 +3352,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6">
       <c r="A58" s="4" t="s">
         <v>133</v>
       </c>
@@ -3360,7 +3366,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6">
       <c r="A59" s="4" t="s">
         <v>133</v>
       </c>
@@ -3374,7 +3380,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6">
       <c r="A60" s="4" t="s">
         <v>133</v>
       </c>
@@ -3388,7 +3394,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6">
       <c r="A61" s="4" t="s">
         <v>134</v>
       </c>
@@ -3402,7 +3408,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6">
       <c r="A62" s="4" t="s">
         <v>134</v>
       </c>
@@ -3416,7 +3422,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6">
       <c r="A63" s="4" t="s">
         <v>134</v>
       </c>
@@ -3430,7 +3436,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6">
       <c r="A64" s="4" t="s">
         <v>134</v>
       </c>
@@ -3444,7 +3450,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6">
       <c r="A65" s="4" t="s">
         <v>134</v>
       </c>
@@ -3458,7 +3464,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6">
       <c r="A66" s="4" t="s">
         <v>134</v>
       </c>
@@ -3472,7 +3478,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6">
       <c r="A67" s="4" t="s">
         <v>134</v>
       </c>
@@ -3486,7 +3492,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6">
       <c r="A68" s="4" t="s">
         <v>134</v>
       </c>
@@ -3500,7 +3506,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="42.75">
       <c r="A69" s="4" t="s">
         <v>134</v>
       </c>
@@ -3514,7 +3520,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6">
       <c r="A70" s="4" t="s">
         <v>134</v>
       </c>
@@ -3528,7 +3534,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6">
       <c r="A71" s="4" t="s">
         <v>134</v>
       </c>
@@ -3542,7 +3548,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6">
       <c r="A72" s="4" t="s">
         <v>134</v>
       </c>
@@ -3556,7 +3562,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6">
       <c r="A73" s="4" t="s">
         <v>134</v>
       </c>
@@ -3570,7 +3576,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6">
       <c r="A74" s="4" t="s">
         <v>134</v>
       </c>
@@ -3584,7 +3590,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6">
       <c r="A75" s="4" t="s">
         <v>134</v>
       </c>
@@ -3598,7 +3604,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" ht="28.5">
       <c r="A76" s="4" t="s">
         <v>134</v>
       </c>
@@ -3612,7 +3618,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6">
       <c r="A77" s="4" t="s">
         <v>134</v>
       </c>
@@ -3626,7 +3632,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6">
       <c r="A78" s="4" t="s">
         <v>134</v>
       </c>
@@ -3640,7 +3646,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6">
       <c r="A79" s="4" t="s">
         <v>134</v>
       </c>
@@ -3654,7 +3660,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6">
       <c r="A80" s="4" t="s">
         <v>134</v>
       </c>
@@ -3668,7 +3674,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6">
       <c r="A81" s="4" t="s">
         <v>134</v>
       </c>
@@ -3682,7 +3688,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6">
       <c r="A82" s="4" t="s">
         <v>135</v>
       </c>
@@ -3696,7 +3702,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="28.5">
       <c r="A83" s="4" t="s">
         <v>135</v>
       </c>
@@ -3710,7 +3716,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6">
       <c r="A84" s="4" t="s">
         <v>135</v>
       </c>
@@ -3724,7 +3730,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6">
       <c r="A85" s="4" t="s">
         <v>135</v>
       </c>
@@ -3738,7 +3744,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6">
       <c r="A86" s="4" t="s">
         <v>135</v>
       </c>
@@ -3752,7 +3758,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="28.5">
       <c r="A87" s="4" t="s">
         <v>135</v>
       </c>
@@ -3766,7 +3772,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6">
       <c r="A88" s="4" t="s">
         <v>135</v>
       </c>
@@ -3780,7 +3786,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6">
       <c r="A89" s="4" t="s">
         <v>135</v>
       </c>
@@ -3794,7 +3800,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6">
       <c r="A90" s="4" t="s">
         <v>135</v>
       </c>
@@ -3808,7 +3814,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6">
       <c r="A91" s="4" t="s">
         <v>135</v>
       </c>
@@ -3822,7 +3828,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6">
       <c r="A92" s="4" t="s">
         <v>135</v>
       </c>
@@ -3836,7 +3842,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6">
       <c r="A93" s="4" t="s">
         <v>135</v>
       </c>
@@ -3850,7 +3856,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6">
       <c r="A94" s="4" t="s">
         <v>135</v>
       </c>
@@ -3864,7 +3870,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6">
       <c r="A95" s="4" t="s">
         <v>135</v>
       </c>
@@ -3878,7 +3884,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6">
       <c r="A96" s="4" t="s">
         <v>135</v>
       </c>
@@ -3892,7 +3898,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="28.5">
       <c r="A97" s="4" t="s">
         <v>135</v>
       </c>
@@ -3906,7 +3912,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6">
       <c r="A98" s="4" t="s">
         <v>135</v>
       </c>
@@ -3920,7 +3926,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="42.75">
       <c r="A99" s="4" t="s">
         <v>135</v>
       </c>
@@ -3934,7 +3940,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6">
       <c r="A100" s="4" t="s">
         <v>135</v>
       </c>
@@ -3948,7 +3954,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6">
       <c r="A101" s="4" t="s">
         <v>135</v>
       </c>
@@ -3962,7 +3968,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="28.5">
       <c r="A102" s="4" t="s">
         <v>135</v>
       </c>
@@ -3976,7 +3982,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6">
       <c r="A103" s="4" t="s">
         <v>135</v>
       </c>
@@ -3990,7 +3996,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6">
       <c r="A104" s="4" t="s">
         <v>135</v>
       </c>
@@ -4004,7 +4010,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6">
       <c r="A105" s="4" t="s">
         <v>135</v>
       </c>
@@ -4018,7 +4024,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="28.5">
       <c r="A106" s="4" t="s">
         <v>135</v>
       </c>
@@ -4032,7 +4038,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="42.75">
       <c r="A107" s="4" t="s">
         <v>135</v>
       </c>
@@ -4046,7 +4052,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="42.75">
       <c r="A108" s="4" t="s">
         <v>135</v>
       </c>
@@ -4060,7 +4066,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="57">
       <c r="A109" s="4" t="s">
         <v>135</v>
       </c>
@@ -4074,7 +4080,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" ht="42.75">
       <c r="A110" s="4" t="s">
         <v>135</v>
       </c>
@@ -4088,7 +4094,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="42.75">
       <c r="A111" s="4" t="s">
         <v>135</v>
       </c>
@@ -4102,7 +4108,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="28.5">
       <c r="A112" s="4" t="s">
         <v>135</v>
       </c>
@@ -4116,7 +4122,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6">
       <c r="A113" s="4" t="s">
         <v>342</v>
       </c>
@@ -4130,7 +4136,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6">
       <c r="A114" s="4" t="s">
         <v>342</v>
       </c>
@@ -4144,7 +4150,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6">
       <c r="A115" s="4" t="s">
         <v>342</v>
       </c>
@@ -4158,7 +4164,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="28.5">
       <c r="A116" s="4" t="s">
         <v>342</v>
       </c>
@@ -4172,7 +4178,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="28.5">
       <c r="A117" s="4" t="s">
         <v>342</v>
       </c>
@@ -4186,7 +4192,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="42.75">
       <c r="A118" s="4" t="s">
         <v>342</v>
       </c>
@@ -4200,7 +4206,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="57">
       <c r="A119" s="4" t="s">
         <v>342</v>
       </c>
@@ -4214,7 +4220,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="28.5">
       <c r="A120" s="4" t="s">
         <v>342</v>
       </c>
@@ -4228,7 +4234,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="71.25">
       <c r="A121" s="4" t="s">
         <v>354</v>
       </c>
@@ -4239,7 +4245,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="42.75">
       <c r="A122" s="4" t="s">
         <v>354</v>
       </c>
@@ -4250,7 +4256,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="71.25">
       <c r="A123" s="4" t="s">
         <v>354</v>
       </c>
@@ -4261,7 +4267,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="71.25">
       <c r="A124" s="4" t="s">
         <v>354</v>
       </c>
@@ -4272,7 +4278,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="57">
       <c r="A125" s="4" t="s">
         <v>354</v>
       </c>
@@ -4286,7 +4292,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="57">
       <c r="A126" s="4" t="s">
         <v>354</v>
       </c>
@@ -4300,7 +4306,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="42.75">
       <c r="A127" s="4" t="s">
         <v>354</v>
       </c>
@@ -4314,7 +4320,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="114">
       <c r="A128" s="4" t="s">
         <v>354</v>
       </c>
@@ -4328,7 +4334,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="28.5">
       <c r="A129" s="4" t="s">
         <v>354</v>
       </c>
@@ -4342,7 +4348,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5">
       <c r="A130" s="4" t="s">
         <v>354</v>
       </c>
@@ -4356,7 +4362,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5">
       <c r="A131" s="4" t="s">
         <v>354</v>
       </c>
@@ -4370,7 +4376,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="28.5">
       <c r="A132" s="4" t="s">
         <v>354</v>
       </c>
@@ -4384,7 +4390,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" ht="42.75">
       <c r="A133" s="4" t="s">
         <v>354</v>
       </c>
@@ -4398,7 +4404,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" ht="71.25">
       <c r="A134" s="4" t="s">
         <v>354</v>
       </c>
@@ -4412,7 +4418,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="28.5">
       <c r="A135" s="4" t="s">
         <v>354</v>
       </c>
@@ -4426,7 +4432,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="28.5">
       <c r="A136" s="4" t="s">
         <v>354</v>
       </c>
@@ -4440,7 +4446,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" ht="71.25">
       <c r="A137" s="4" t="s">
         <v>354</v>
       </c>
@@ -4454,7 +4460,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" ht="42.75">
       <c r="A138" s="4" t="s">
         <v>354</v>
       </c>
@@ -4468,7 +4474,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" ht="57">
       <c r="A139" s="4" t="s">
         <v>354</v>
       </c>
@@ -4485,7 +4491,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" ht="28.5">
       <c r="A140" s="4" t="s">
         <v>354</v>
       </c>
@@ -4502,7 +4508,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="28.5">
       <c r="A141" s="4" t="s">
         <v>354</v>
       </c>
@@ -4519,7 +4525,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" ht="42.75">
       <c r="A142" s="4" t="s">
         <v>354</v>
       </c>
@@ -4536,7 +4542,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" ht="28.5">
       <c r="A143" s="4" t="s">
         <v>354</v>
       </c>
@@ -4553,7 +4559,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="28.5">
       <c r="A144" s="4" t="s">
         <v>354</v>
       </c>
@@ -4570,7 +4576,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" ht="57">
       <c r="A145" s="4" t="s">
         <v>354</v>
       </c>
@@ -4584,7 +4590,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" ht="28.5">
       <c r="A146" s="4" t="s">
         <v>374</v>
       </c>
@@ -4594,8 +4600,11 @@
       <c r="E146" s="2" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F146" s="2" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" ht="28.5">
       <c r="A147" s="4" t="s">
         <v>374</v>
       </c>
@@ -4604,6 +4613,9 @@
       </c>
       <c r="E147" s="2" t="s">
         <v>402</v>
+      </c>
+      <c r="F147" s="2" t="s">
+        <v>503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spanish interface language, bugfixes
</commit_message>
<xml_diff>
--- a/docs/CMDI Maker Localisations.xlsx
+++ b/docs/CMDI Maker Localisations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="585"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="588"/>
   </bookViews>
   <sheets>
     <sheet name="APP CORE" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="543">
   <si>
     <t>Key1</t>
   </si>
@@ -1537,6 +1537,135 @@
   </si>
   <si>
     <t>Der komplette und ausführliche Titel deines Korpus.</t>
+  </si>
+  <si>
+    <t>Esta opción elimina todos los datos que CMDI Maker ha almacenado en su ordenador.</t>
+  </si>
+  <si>
+    <t>Lenguaje del programa</t>
+  </si>
+  <si>
+    <t>¡No se encontró ningún dato para CMDI Maker en el archivo!</t>
+  </si>
+  <si>
+    <t>No se encontró ningún dato para el perfíl activo</t>
+  </si>
+  <si>
+    <t>Formulario guardado</t>
+  </si>
+  <si>
+    <t>Sí, eliminar todo</t>
+  </si>
+  <si>
+    <t>Sí, sobrescribir los datos</t>
+  </si>
+  <si>
+    <t>¿Quiere realmente sobrescribir todos los datos?</t>
+  </si>
+  <si>
+    <t>¿Quieres realmente resetear CMDI Maker por completo? ¡Todos los datos serán eliminados!</t>
+  </si>
+  <si>
+    <t>Encendido</t>
+  </si>
+  <si>
+    <t>Apagado</t>
+  </si>
+  <si>
+    <t>¡Bienvenido de nuevo!</t>
+  </si>
+  <si>
+    <t>Acerca de</t>
+  </si>
+  <si>
+    <t>Guardar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bienvenidos al CMDI Maker!&lt;br&gt;Fígese, ésta es una aplicación que se puede utilizar también sin conexión.&lt;br&gt;Cuando cargue esta página, podrá reanudar su trabajo en el punto donde lo interrumpió. </t>
+  </si>
+  <si>
+    <t>¡y vamos a empezar!</t>
+  </si>
+  <si>
+    <t>CMDI Maker está financiado por</t>
+  </si>
+  <si>
+    <t>¿Necesita ayuda?</t>
+  </si>
+  <si>
+    <t>En las páginas de ayuda encontrará videos tutoriales, una lista de correo electrónico y de personas para consultar en caso de necesidad, ¡y mucho más!</t>
+  </si>
+  <si>
+    <t>Seleccione su perfíl</t>
+  </si>
+  <si>
+    <t>Esto es</t>
+  </si>
+  <si>
+    <t>Configuración</t>
+  </si>
+  <si>
+    <t>Perfíl</t>
+  </si>
+  <si>
+    <t>Guardar automáticamente</t>
+  </si>
+  <si>
+    <t>Cada 30 segundos</t>
+  </si>
+  <si>
+    <t>Cada 60 segundos</t>
+  </si>
+  <si>
+    <t>Cada 5 minutos</t>
+  </si>
+  <si>
+    <t>Cada 10 minutos</t>
+  </si>
+  <si>
+    <t>Lenguaje Global de Metadatos</t>
+  </si>
+  <si>
+    <t>Creador de Metadatos CMDI</t>
+  </si>
+  <si>
+    <t>El formato de metadatos CMDI requiere el nombre de un creador de metadatos. Éste, probablemente, es usted. Si lo es, escriba su nombre.</t>
+  </si>
+  <si>
+    <t>Guardar proyecto</t>
+  </si>
+  <si>
+    <t>Con esta opción todos sus datos serán guardados en un solo archivo. Este archivo podrá luego ser importado otra vez por CMDI Maker.</t>
+  </si>
+  <si>
+    <t>Cargar proyecto</t>
+  </si>
+  <si>
+    <t>Esta opción carga un archivo CMP (CMDI Maker Project) junto con los datos del proyecto.</t>
+  </si>
+  <si>
+    <t>CMDI Maker guarda los datos que se introducen en la base de datos de un navegador, y los guardará aun cuando se cierre el navegador.&lt;br&gt;De todas formas, si la opción Guardar automáticamente está seleccionada, los nuevos datos serán guardados automáticamente.&lt;br&gt;¡Esta función elimina solamente los datos pertenecientes al perfil activo!</t>
+  </si>
+  <si>
+    <t>Reseteo completo</t>
+  </si>
+  <si>
+    <t>Español (id: "spanish")</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">English (id: "english")
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>This is the reference language. Translations should always take this language as source.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1546,7 +1675,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1567,8 +1696,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1584,6 +1719,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1615,7 +1762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1625,6 +1772,12 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1905,27 +2058,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="4"/>
+    <col min="1" max="1" width="11.44140625" style="4"/>
     <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="4"/>
-    <col min="5" max="5" width="30.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="4"/>
+    <col min="5" max="5" width="31" style="2" customWidth="1"/>
     <col min="6" max="6" width="32" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="26.625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.5" style="2"/>
+    <col min="7" max="7" width="31.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1938,14 +2091,17 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>95</v>
+      <c r="E1" s="6" t="s">
+        <v>542</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -1958,8 +2114,11 @@
       <c r="F2" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" s="2" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1972,8 +2131,11 @@
       <c r="F3" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -1986,8 +2148,11 @@
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" s="2" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2000,8 +2165,11 @@
       <c r="F5" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -2014,8 +2182,11 @@
       <c r="F6" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" s="2" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2028,8 +2199,11 @@
       <c r="F7" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" s="2" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -2042,8 +2216,11 @@
       <c r="F8" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" s="2" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -2056,8 +2233,11 @@
       <c r="F9" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" s="2" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -2070,8 +2250,11 @@
       <c r="F10" s="2" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" s="2" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -2084,8 +2267,11 @@
       <c r="F11" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="57">
+      <c r="G11" s="2" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -2098,8 +2284,11 @@
       <c r="F12" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" s="2" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -2112,8 +2301,11 @@
       <c r="F13" s="2" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="57">
+      <c r="G13" s="2" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -2126,8 +2318,11 @@
       <c r="F14" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" s="2" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -2140,8 +2335,11 @@
       <c r="F15" s="2" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="28.5">
+      <c r="G15" s="2" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -2154,8 +2352,11 @@
       <c r="F16" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16" s="2" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -2168,8 +2369,9 @@
       <c r="F17" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="156.75">
+      <c r="G17" s="5"/>
+    </row>
+    <row r="18" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -2182,8 +2384,11 @@
       <c r="F18" s="2" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" s="2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
@@ -2196,8 +2401,11 @@
       <c r="F19" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="42.75">
+      <c r="G19" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
@@ -2210,8 +2418,11 @@
       <c r="F20" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" s="2" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -2224,8 +2435,11 @@
       <c r="F21" s="2" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="28.5">
+      <c r="G21" s="2" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -2238,8 +2452,11 @@
       <c r="F22" s="2" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" s="2" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
@@ -2252,8 +2469,9 @@
       <c r="F23" s="2" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.5">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
@@ -2266,8 +2484,11 @@
       <c r="F24" s="2" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>50</v>
       </c>
@@ -2280,8 +2501,11 @@
       <c r="F25" s="2" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" s="2" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>54</v>
       </c>
@@ -2294,8 +2518,11 @@
       <c r="F26" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
@@ -2308,8 +2535,11 @@
       <c r="F27" s="2" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
@@ -2322,8 +2552,11 @@
       <c r="F28" s="2" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="28.5">
+      <c r="G28" s="2" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>54</v>
       </c>
@@ -2336,8 +2569,11 @@
       <c r="F29" s="2" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="42.75">
+      <c r="G29" s="2" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>54</v>
       </c>
@@ -2350,8 +2586,11 @@
       <c r="F30" s="2" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="2" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>65</v>
       </c>
@@ -2361,8 +2600,11 @@
       <c r="F31" s="2" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" s="2" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>11</v>
       </c>
@@ -2372,8 +2614,11 @@
       <c r="F32" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="2" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>66</v>
       </c>
@@ -2383,8 +2628,11 @@
       <c r="F33" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>69</v>
       </c>
@@ -2394,8 +2642,11 @@
       <c r="F34" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34" s="2" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>71</v>
       </c>
@@ -2405,8 +2656,11 @@
       <c r="F35" s="2" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>72</v>
       </c>
@@ -2416,8 +2670,11 @@
       <c r="F36" s="2" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="99.75">
+      <c r="G36" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>75</v>
       </c>
@@ -2430,8 +2687,11 @@
       <c r="F37" s="2" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37" s="2" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>75</v>
       </c>
@@ -2444,8 +2704,11 @@
       <c r="F38" s="2" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38" s="2" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>75</v>
       </c>
@@ -2458,8 +2721,11 @@
       <c r="F39" s="2" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39" s="2" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>75</v>
       </c>
@@ -2472,8 +2738,11 @@
       <c r="F40" s="2" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="57">
+      <c r="G40" s="2" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>75</v>
       </c>
@@ -2486,8 +2755,11 @@
       <c r="F41" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="G41" s="2" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>75</v>
       </c>
@@ -2500,8 +2772,11 @@
       <c r="F42" s="2" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42" s="2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>75</v>
       </c>
@@ -2517,8 +2792,11 @@
       <c r="F43" s="2" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>75</v>
       </c>
@@ -2532,6 +2810,9 @@
         <v>92</v>
       </c>
       <c r="F44" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2550,20 +2831,20 @@
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="4"/>
+    <col min="1" max="1" width="11.44140625" style="4"/>
     <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="4"/>
-    <col min="5" max="5" width="30.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="4"/>
+    <col min="5" max="5" width="30.44140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="32" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="26.625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.5" style="2"/>
+    <col min="7" max="7" width="31.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2583,7 +2864,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>131</v>
       </c>
@@ -2597,7 +2878,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>131</v>
       </c>
@@ -2611,7 +2892,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>131</v>
       </c>
@@ -2625,7 +2906,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>131</v>
       </c>
@@ -2639,7 +2920,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>131</v>
       </c>
@@ -2653,7 +2934,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.5">
+    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2667,7 +2948,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="156.75">
+    <row r="8" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -2681,7 +2962,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -2695,7 +2976,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -2709,7 +2990,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -2723,7 +3004,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -2737,7 +3018,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.5">
+    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -2751,7 +3032,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="28.5">
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -2765,7 +3046,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -2779,7 +3060,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="71.25">
+    <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -2793,7 +3074,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>147</v>
       </c>
@@ -2804,7 +3085,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>148</v>
       </c>
@@ -2815,7 +3096,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>55</v>
       </c>
@@ -2826,7 +3107,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="42.75">
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>149</v>
       </c>
@@ -2837,7 +3118,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>150</v>
       </c>
@@ -2848,7 +3129,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>151</v>
       </c>
@@ -2859,7 +3140,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>66</v>
       </c>
@@ -2870,7 +3151,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="28.5">
+    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>152</v>
       </c>
@@ -2881,7 +3162,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28.5">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>174</v>
       </c>
@@ -2895,7 +3176,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>174</v>
       </c>
@@ -2909,7 +3190,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>174</v>
       </c>
@@ -2923,7 +3204,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>174</v>
       </c>
@@ -2937,7 +3218,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>174</v>
       </c>
@@ -2951,7 +3232,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>174</v>
       </c>
@@ -2965,7 +3246,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>174</v>
       </c>
@@ -2979,7 +3260,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>174</v>
       </c>
@@ -2993,7 +3274,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>174</v>
       </c>
@@ -3007,7 +3288,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="42.75">
+    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>174</v>
       </c>
@@ -3021,7 +3302,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>174</v>
       </c>
@@ -3035,7 +3316,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>174</v>
       </c>
@@ -3049,7 +3330,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>174</v>
       </c>
@@ -3063,7 +3344,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>174</v>
       </c>
@@ -3077,7 +3358,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>174</v>
       </c>
@@ -3091,7 +3372,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="42.75">
+    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>133</v>
       </c>
@@ -3108,7 +3389,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="57">
+    <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>133</v>
       </c>
@@ -3125,7 +3406,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="57">
+    <row r="42" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>133</v>
       </c>
@@ -3142,7 +3423,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>133</v>
       </c>
@@ -3156,7 +3437,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>133</v>
       </c>
@@ -3170,7 +3451,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>133</v>
       </c>
@@ -3184,7 +3465,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>133</v>
       </c>
@@ -3198,7 +3479,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>133</v>
       </c>
@@ -3212,7 +3493,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>133</v>
       </c>
@@ -3226,7 +3507,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>133</v>
       </c>
@@ -3240,7 +3521,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>133</v>
       </c>
@@ -3254,7 +3535,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>133</v>
       </c>
@@ -3268,7 +3549,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>133</v>
       </c>
@@ -3282,7 +3563,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="28.5">
+    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>133</v>
       </c>
@@ -3296,7 +3577,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>133</v>
       </c>
@@ -3310,7 +3591,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="28.5">
+    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>133</v>
       </c>
@@ -3324,7 +3605,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>133</v>
       </c>
@@ -3338,7 +3619,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="28.5">
+    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>133</v>
       </c>
@@ -3352,7 +3633,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>133</v>
       </c>
@@ -3366,7 +3647,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>133</v>
       </c>
@@ -3380,7 +3661,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>133</v>
       </c>
@@ -3394,7 +3675,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>134</v>
       </c>
@@ -3408,7 +3689,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>134</v>
       </c>
@@ -3422,7 +3703,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>134</v>
       </c>
@@ -3436,7 +3717,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>134</v>
       </c>
@@ -3450,7 +3731,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>134</v>
       </c>
@@ -3464,7 +3745,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>134</v>
       </c>
@@ -3478,7 +3759,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>134</v>
       </c>
@@ -3492,7 +3773,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>134</v>
       </c>
@@ -3506,7 +3787,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="42.75">
+    <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>134</v>
       </c>
@@ -3520,7 +3801,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>134</v>
       </c>
@@ -3534,7 +3815,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>134</v>
       </c>
@@ -3548,7 +3829,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>134</v>
       </c>
@@ -3562,7 +3843,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>134</v>
       </c>
@@ -3576,7 +3857,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>134</v>
       </c>
@@ -3590,7 +3871,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>134</v>
       </c>
@@ -3604,7 +3885,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="28.5">
+    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>134</v>
       </c>
@@ -3618,7 +3899,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>134</v>
       </c>
@@ -3632,7 +3913,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>134</v>
       </c>
@@ -3646,7 +3927,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>134</v>
       </c>
@@ -3660,7 +3941,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>134</v>
       </c>
@@ -3674,7 +3955,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>134</v>
       </c>
@@ -3688,7 +3969,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>135</v>
       </c>
@@ -3702,7 +3983,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="28.5">
+    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>135</v>
       </c>
@@ -3716,7 +3997,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>135</v>
       </c>
@@ -3730,7 +4011,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>135</v>
       </c>
@@ -3744,7 +4025,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>135</v>
       </c>
@@ -3758,7 +4039,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="28.5">
+    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>135</v>
       </c>
@@ -3772,7 +4053,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>135</v>
       </c>
@@ -3786,7 +4067,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>135</v>
       </c>
@@ -3800,7 +4081,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>135</v>
       </c>
@@ -3814,7 +4095,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>135</v>
       </c>
@@ -3828,7 +4109,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>135</v>
       </c>
@@ -3842,7 +4123,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>135</v>
       </c>
@@ -3856,7 +4137,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>135</v>
       </c>
@@ -3870,7 +4151,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>135</v>
       </c>
@@ -3884,7 +4165,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>135</v>
       </c>
@@ -3898,7 +4179,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="28.5">
+    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>135</v>
       </c>
@@ -3912,7 +4193,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>135</v>
       </c>
@@ -3926,7 +4207,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="42.75">
+    <row r="99" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>135</v>
       </c>
@@ -3940,7 +4221,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>135</v>
       </c>
@@ -3954,7 +4235,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>135</v>
       </c>
@@ -3968,7 +4249,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="28.5">
+    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>135</v>
       </c>
@@ -3982,7 +4263,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>135</v>
       </c>
@@ -3996,7 +4277,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>135</v>
       </c>
@@ -4010,7 +4291,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>135</v>
       </c>
@@ -4024,7 +4305,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="28.5">
+    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>135</v>
       </c>
@@ -4038,7 +4319,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="42.75">
+    <row r="107" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>135</v>
       </c>
@@ -4052,7 +4333,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="42.75">
+    <row r="108" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>135</v>
       </c>
@@ -4066,7 +4347,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="57">
+    <row r="109" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>135</v>
       </c>
@@ -4080,7 +4361,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="42.75">
+    <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>135</v>
       </c>
@@ -4094,7 +4375,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="42.75">
+    <row r="111" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>135</v>
       </c>
@@ -4108,7 +4389,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="28.5">
+    <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>135</v>
       </c>
@@ -4122,7 +4403,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>342</v>
       </c>
@@ -4136,7 +4417,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>342</v>
       </c>
@@ -4150,7 +4431,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>342</v>
       </c>
@@ -4164,7 +4445,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="28.5">
+    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>342</v>
       </c>
@@ -4178,7 +4459,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="28.5">
+    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>342</v>
       </c>
@@ -4192,7 +4473,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="42.75">
+    <row r="118" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>342</v>
       </c>
@@ -4206,7 +4487,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="57">
+    <row r="119" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>342</v>
       </c>
@@ -4220,7 +4501,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="28.5">
+    <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>342</v>
       </c>
@@ -4234,7 +4515,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="71.25">
+    <row r="121" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>354</v>
       </c>
@@ -4245,7 +4526,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="42.75">
+    <row r="122" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>354</v>
       </c>
@@ -4256,7 +4537,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="71.25">
+    <row r="123" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>354</v>
       </c>
@@ -4267,7 +4548,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="71.25">
+    <row r="124" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>354</v>
       </c>
@@ -4278,7 +4559,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="57">
+    <row r="125" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
         <v>354</v>
       </c>
@@ -4292,7 +4573,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="57">
+    <row r="126" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
         <v>354</v>
       </c>
@@ -4306,7 +4587,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="42.75">
+    <row r="127" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
         <v>354</v>
       </c>
@@ -4320,7 +4601,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="114">
+    <row r="128" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
         <v>354</v>
       </c>
@@ -4334,7 +4615,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="28.5">
+    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
         <v>354</v>
       </c>
@@ -4348,7 +4629,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>354</v>
       </c>
@@ -4362,7 +4643,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>354</v>
       </c>
@@ -4376,7 +4657,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="28.5">
+    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>354</v>
       </c>
@@ -4390,7 +4671,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="42.75">
+    <row r="133" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>354</v>
       </c>
@@ -4404,7 +4685,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="71.25">
+    <row r="134" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>354</v>
       </c>
@@ -4418,7 +4699,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="28.5">
+    <row r="135" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
         <v>354</v>
       </c>
@@ -4432,7 +4713,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="28.5">
+    <row r="136" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>354</v>
       </c>
@@ -4446,7 +4727,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="71.25">
+    <row r="137" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
         <v>354</v>
       </c>
@@ -4460,7 +4741,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="42.75">
+    <row r="138" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>354</v>
       </c>
@@ -4474,7 +4755,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="57">
+    <row r="139" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
         <v>354</v>
       </c>
@@ -4491,7 +4772,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="140" spans="1:5" ht="28.5">
+    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
         <v>354</v>
       </c>
@@ -4508,7 +4789,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="28.5">
+    <row r="141" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
         <v>354</v>
       </c>
@@ -4525,7 +4806,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="142" spans="1:5" ht="42.75">
+    <row r="142" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
         <v>354</v>
       </c>
@@ -4542,7 +4823,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="143" spans="1:5" ht="28.5">
+    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
         <v>354</v>
       </c>
@@ -4559,7 +4840,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="28.5">
+    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>354</v>
       </c>
@@ -4576,7 +4857,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="145" spans="1:6" ht="57">
+    <row r="145" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
         <v>354</v>
       </c>
@@ -4590,7 +4871,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="146" spans="1:6" ht="28.5">
+    <row r="146" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="4" t="s">
         <v>374</v>
       </c>
@@ -4604,7 +4885,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="28.5">
+    <row r="147" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
         <v>374</v>
       </c>

</xml_diff>

<commit_message>
IMDI: Added Spanish LanguagePack, Bugfixes
</commit_message>
<xml_diff>
--- a/docs/CMDI Maker Localisations.xlsx
+++ b/docs/CMDI Maker Localisations.xlsx
@@ -15,7 +15,7 @@
     <sheet name="APP CORE" sheetId="1" r:id="rId1"/>
     <sheet name="IMDI" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="701">
   <si>
     <t>Key1</t>
   </si>
@@ -1666,6 +1666,480 @@
       </rPr>
       <t>This is the reference language. Translations should always take this language as source.</t>
     </r>
+  </si>
+  <si>
+    <t>Recursos</t>
+  </si>
+  <si>
+    <t>Actores</t>
+  </si>
+  <si>
+    <t>Sesiones</t>
+  </si>
+  <si>
+    <t>Calcular la edad del actor</t>
+  </si>
+  <si>
+    <t>Cuando esta función está activada, CMDI Maker controla si la edad del actor (si ésta no ha sido especificada todavía) puede ser calculada a través de la fecha de nacimiento del actor y de la fecha de la sesión.&lt;br&gt;Si la edad puede ser calculada, ésta aparecerá en el archivo de salida.&lt;br&gt;(Edad = Fecha de la sesión - Fecha de nacimiento del actor)</t>
+  </si>
+  <si>
+    <t>Formato del archivo de salida</t>
+  </si>
+  <si>
+    <t>CMDI con perfíl IMDI</t>
+  </si>
+  <si>
+    <t>Exportar actores como JSON</t>
+  </si>
+  <si>
+    <t>Importar actores desde JSON o IMDI</t>
+  </si>
+  <si>
+    <t>¡Por favor importar solamente archivos codificados en UTF-8!</t>
+  </si>
+  <si>
+    <t>Eliminar actores</t>
+  </si>
+  <si>
+    <t>CMDI Maker guarda todos sus actores en una base de datos de Web Storage, así que éstos quedarán guardados aun si se cierra la ventana del navegador.</t>
+  </si>
+  <si>
+    <t>Resetear formulario</t>
+  </si>
+  <si>
+    <t>Sí, eliminar formulario</t>
+  </si>
+  <si>
+    <t>¿Quieres realmente resetear el formulario y eliminar el corpus y todas sus sesiones?</t>
+  </si>
+  <si>
+    <t>Reseteo del formulario</t>
+  </si>
+  <si>
+    <t>Buscar</t>
+  </si>
+  <si>
+    <t>¡Esta función no está actualmente disponible!</t>
+  </si>
+  <si>
+    <t>Establecer Content Language global</t>
+  </si>
+  <si>
+    <t>o bien ingresar un código ISO</t>
+  </si>
+  <si>
+    <t>Buscar lengua</t>
+  </si>
+  <si>
+    <t>resultado</t>
+  </si>
+  <si>
+    <t>resultados</t>
+  </si>
+  <si>
+    <t>Nombre de la lengua</t>
+  </si>
+  <si>
+    <t>es un nuevo Content Language global</t>
+  </si>
+  <si>
+    <t>Código ISO</t>
+  </si>
+  <si>
+    <t>no se encontró en la base de datos</t>
+  </si>
+  <si>
+    <t>Por favor especifique su búsqueda.\nIngrese por lo menos 3 caracteres.</t>
+  </si>
+  <si>
+    <t>Lengua principal</t>
+  </si>
+  <si>
+    <t>Lengua materna</t>
+  </si>
+  <si>
+    <t>Content Languages corrientes</t>
+  </si>
+  <si>
+    <t>" eliminada</t>
+  </si>
+  <si>
+    <t>Este archivo multimedia no es un archivo  de recursos válido para LAMUS. Por favor intente convertir su código.</t>
+  </si>
+  <si>
+    <t>Desconocido</t>
+  </si>
+  <si>
+    <t>Crear una sesión para cada archivo</t>
+  </si>
+  <si>
+    <t>Archivos</t>
+  </si>
+  <si>
+    <t>Archivos seleccionados</t>
+  </si>
+  <si>
+    <t>Ordenar los archivo alfabéticamente</t>
+  </si>
+  <si>
+    <t>Eliminar</t>
+  </si>
+  <si>
+    <t>Quitar lista de archivos</t>
+  </si>
+  <si>
+    <t>Arrastrar y soltar los archivos aquí</t>
+  </si>
+  <si>
+    <t>Uso</t>
+  </si>
+  <si>
+    <t>Pulsar</t>
+  </si>
+  <si>
+    <t>Seleccionar recurso, pulsar otra vez para deseleccionar un solo recurso</t>
+  </si>
+  <si>
+    <t>Mantener pulsada la tecla Shift para seleccionar varios recursos</t>
+  </si>
+  <si>
+    <t>Pulsar escape para deseleccionar todos los recursos</t>
+  </si>
+  <si>
+    <t>Tamaño</t>
+  </si>
+  <si>
+    <t>Modificado la última vez</t>
+  </si>
+  <si>
+    <t>No se importó ningún archivo de recursos.</t>
+  </si>
+  <si>
+    <t>Nuevo actor</t>
+  </si>
+  <si>
+    <t>Eliminar este actor</t>
+  </si>
+  <si>
+    <t>Ordenar actores alfabéticamente</t>
+  </si>
+  <si>
+    <t>Actores ordenados</t>
+  </si>
+  <si>
+    <t>Guardar y duplicar este actor</t>
+  </si>
+  <si>
+    <t>Sí, eliminar todos los actores</t>
+  </si>
+  <si>
+    <t>¿Quiere realmente eliminar la base de datos de los actores por completo?</t>
+  </si>
+  <si>
+    <t>Se eliminaron todos los actores</t>
+  </si>
+  <si>
+    <t>Guardar actor</t>
+  </si>
+  <si>
+    <t>Guardar los cambios hechos a este actor</t>
+  </si>
+  <si>
+    <t>¡No hay actores!</t>
+  </si>
+  <si>
+    <t>se importaron los actores</t>
+  </si>
+  <si>
+    <t>Actor guardado y duplicado.</t>
+  </si>
+  <si>
+    <t>Por favor, primero dé un nombre a su actor.</t>
+  </si>
+  <si>
+    <t>Sí, eliminar actor</t>
+  </si>
+  <si>
+    <t>¿Quiere realmente eliminar</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> eliminado</t>
+  </si>
+  <si>
+    <t>Nueva sesión</t>
+  </si>
+  <si>
+    <t>Copiar los metadatos de la Sesión 1 a todas las sesiones</t>
+  </si>
+  <si>
+    <t>Ordenar según el nombre</t>
+  </si>
+  <si>
+    <t>Añadir a la sesión</t>
+  </si>
+  <si>
+    <t>No se añadió ningún archivo.</t>
+  </si>
+  <si>
+    <t>Añadir unos archivos.</t>
+  </si>
+  <si>
+    <t>Se creó una nueva sesión.</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Sesión sin nombre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sesión </t>
+  </si>
+  <si>
+    <t>Eliminar sesión</t>
+  </si>
+  <si>
+    <t>Extender sesión</t>
+  </si>
+  <si>
+    <t>Doblar sesión</t>
+  </si>
+  <si>
+    <t>Extender/doblar sesión</t>
+  </si>
+  <si>
+    <t>Todavía no hay actores en la base de datos.</t>
+  </si>
+  <si>
+    <t>Crear unos actores.</t>
+  </si>
+  <si>
+    <t>¿Quiere realmente eliminar una sesión entera? Está seguro?</t>
+  </si>
+  <si>
+    <t>Sí, eliminar sesión</t>
+  </si>
+  <si>
+    <t>Sesión eliminada</t>
+  </si>
+  <si>
+    <t>Todavía no hay sesiones en este corpus.</t>
+  </si>
+  <si>
+    <t>crear una</t>
+  </si>
+  <si>
+    <t>Este actor ya está en la sesión.</t>
+  </si>
+  <si>
+    <t>Tenemos un problema.&lt;br&gt;No sé si este archivo es un archivo multimedia o un recurso escrito:</t>
+  </si>
+  <si>
+    <t>Por ahora lo voy a considerar un recurso escrito. Pero no deberías volver a hacerlo.</t>
+  </si>
+  <si>
+    <t>El nombre de la sesión viene del nombre del archivo EAF, porque todavía no se le ha dado ningún nombre.</t>
+  </si>
+  <si>
+    <t>La fecha de la sesión viene del nombre del archivo EAF.</t>
+  </si>
+  <si>
+    <t>Hay que haber por lo menos 2 sesiones para asignar los metadatos de una a otra.</t>
+  </si>
+  <si>
+    <t>Se asignaron los metadatos de la Sesión 1 a todas las sesiones.</t>
+  </si>
+  <si>
+    <t>¡Primero debe crear unas sesiones!</t>
+  </si>
+  <si>
+    <t>¡Cada sesión debe tener un nombre de proyecto!</t>
+  </si>
+  <si>
+    <t>El corpus debe tener un nombre adecuado, o no tener ningún nombre.&lt;br&gt;No se admiten:</t>
+  </si>
+  <si>
+    <t>Cada sesión debe tener un nombre adecuado.&lt;br&gt;Las sesiones sin nombre no están permitidas.&lt;br&gt;No se admiten:</t>
+  </si>
+  <si>
+    <t>Bajar corpus junto con todas las sesiones</t>
+  </si>
+  <si>
+    <t>Un nombre corto o la abreviatura de una o dos palabras. Este identificador permite distinguir una sesión de las otras en el mismo (sub-) corpus y se utiliza para facilitar la navegación.</t>
+  </si>
+  <si>
+    <t>El título de la sesión es el título completo de la sesión sin ninguna abreviatura.</t>
+  </si>
+  <si>
+    <t>En general, la fecha principal de la sesión es la fecha de un archivo audio o video. Si la sesión incluye solamente recursos escritos, ésta indicará la fecha de creación del documento principal.</t>
+  </si>
+  <si>
+    <t>Aquí se puede proporcionar una descripción relacionada con la sesión entera. Ejemplo: Conversación entre la madre, el padre y el hijo a la mesa desayunando.</t>
+  </si>
+  <si>
+    <t>Si el documento está relacionado con "las lenguas de Sur América", se debe especificar solamente la voz Continent.</t>
+  </si>
+  <si>
+    <t>Este elemento se puede utilizar también para describir sub-regiones. Ejemplos: Europa, Paises Bajos, Gelderland, Achterhoek.</t>
+  </si>
+  <si>
+    <t>Por ejemplo si las sesiones de grabación ocurrieron en un instituto, entonces se requiere la dirección de ese instituto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si una sesión se creó dentro de un proyecto, habrá unas informaciones relacionadas con este proyecto. Estas informaciones suelen ser recicladas para varias sesiones y varios corpora si estos pertenecen al mismo proyecto. </t>
+  </si>
+  <si>
+    <t>Un nombre corto o una abreviatura del proyecto.</t>
+  </si>
+  <si>
+    <t>El título completo del proyecto.</t>
+  </si>
+  <si>
+    <t>Un identificador único para el proyecto.</t>
+  </si>
+  <si>
+    <t>Una descripción elaborada del ámbito y de los objetivos del proyecto.</t>
+  </si>
+  <si>
+    <t>Informaciones de contacto de la persona o del instituto responsable del proyecto.</t>
+  </si>
+  <si>
+    <t>El grupo de contenido se usa para describir el contenido de la sesión. Esto se hace a través de cuatro dimensiones (contexto de la comunicación, género, tarea y modalidades).</t>
+  </si>
+  <si>
+    <t>Los tipos de discurso convencionalizados del contenido de la sesión.</t>
+  </si>
+  <si>
+    <t>Los sub-tipos de discurso convencionalizados del contenido de una sesión.</t>
+  </si>
+  <si>
+    <t>En áreas como ingeniería del lenguaje se suelen tener típicas tareas o situaciones como por ejemplo "info kiosk task" o bien "frog story".</t>
+  </si>
+  <si>
+    <t>Por el contrario, el texto en prosa se puede utilizar para describir el contenido.</t>
+  </si>
+  <si>
+    <t>Este grupo de elementos se utiliza para describir el contexto de comunicación en el que se hizo la grabación.</t>
+  </si>
+  <si>
+    <t>Indica la estructura del evento comunicativo.</t>
+  </si>
+  <si>
+    <t>Indica cuanto el consultor planeó el evento lingüístico.</t>
+  </si>
+  <si>
+    <t>Caracteriza el grado de interacción entre todos los actores de la sesión.</t>
+  </si>
+  <si>
+    <t>Indica el contexto social en el que ocurrió el evento.</t>
+  </si>
+  <si>
+    <t>Indica cuanto el investigador estaba involucrado en el evento lingüístico.</t>
+  </si>
+  <si>
+    <t>La descripción se refiere a todos los actores y debería utilizarse para describir las interacciones y las interrelaciones entre los actores.</t>
+  </si>
+  <si>
+    <t>Un nombre corto y archivable de su corpus.</t>
+  </si>
+  <si>
+    <t>El título completo y extenso de su corpus.</t>
+  </si>
+  <si>
+    <t>Eliminar datos guardados</t>
+  </si>
+  <si>
+    <t>Datos pertenecientes al perfíl activo eliminados</t>
+  </si>
+  <si>
+    <t>export_to_file</t>
+  </si>
+  <si>
+    <t>Exportar a archivo</t>
+  </si>
+  <si>
+    <t>In Datei exportieren</t>
+  </si>
+  <si>
+    <t>Export to file</t>
+  </si>
+  <si>
+    <t>Este archivo multimedia no es un archivo  de recursos válido para LAMUS. Por favor intente convertir su código en formato WAV (audio) o en MP4 (video).</t>
+  </si>
+  <si>
+    <t>Este archivo multimedia no es un archivo  de recursos válido para LAMUS. Por favor intente convertir su código en formato PDF o en TXT.</t>
+  </si>
+  <si>
+    <t>duplicate_this_actor</t>
+  </si>
+  <si>
+    <t>Duplicate actor</t>
+  </si>
+  <si>
+    <t>Actor duplizieren</t>
+  </si>
+  <si>
+    <t>Duplicar este actor</t>
+  </si>
+  <si>
+    <t>there_are_no_actors_yet</t>
+  </si>
+  <si>
+    <t>please_give_all_actors_a_name_before_creating_new_one</t>
+  </si>
+  <si>
+    <t>really_erase_this_actor</t>
+  </si>
+  <si>
+    <t>unnamed_actor</t>
+  </si>
+  <si>
+    <t>There are no actors yet.</t>
+  </si>
+  <si>
+    <t>Es gibt noch keine Actors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> du nicht einen?</t>
+  </si>
+  <si>
+    <t>create</t>
+  </si>
+  <si>
+    <t>one?</t>
+  </si>
+  <si>
+    <t>Please give all actors a name before creating a new one.</t>
+  </si>
+  <si>
+    <t>Bitte gib all deinen Actors einen Namen, bevor du einen neuen erstellst!</t>
+  </si>
+  <si>
+    <t>Willst Du diesen Actor wirklich löschen?</t>
+  </si>
+  <si>
+    <t>Unbenannter Actor</t>
+  </si>
+  <si>
+    <t>Do you really want to erase this actor?</t>
+  </si>
+  <si>
+    <t>Unnamed Actor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">¿Porque no </t>
+  </si>
+  <si>
+    <t>download_zip_archive</t>
+  </si>
+  <si>
+    <t>Download ZIP archive</t>
+  </si>
+  <si>
+    <t>ZIP-Archiv herunterladen</t>
   </si>
 </sst>
 </file>
@@ -1703,7 +2177,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1719,12 +2193,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1772,10 +2240,10 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2058,11 +2526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2091,7 +2559,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>542</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -2369,7 +2837,9 @@
       <c r="F17" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="6" t="s">
+        <v>670</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
@@ -2456,7 +2926,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
@@ -2469,7 +2939,9 @@
       <c r="F23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="G23" s="5"/>
+      <c r="G23" s="6" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
@@ -2674,38 +3146,35 @@
         <v>517</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>76</v>
+        <v>672</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>82</v>
+        <v>675</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>125</v>
+        <v>674</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2713,16 +3182,16 @@
         <v>75</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -2730,50 +3199,50 @@
         <v>75</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>75</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
@@ -2781,19 +3250,16 @@
         <v>75</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
@@ -2804,16 +3270,70 @@
         <v>88</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F45" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="G45" s="2" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>559</v>
       </c>
     </row>
   </sheetData>
@@ -2824,11 +3344,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F147"/>
+  <dimension ref="A1:G156"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2844,7 +3364,7 @@
     <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2863,8 +3383,11 @@
       <c r="F1" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>131</v>
       </c>
@@ -2877,8 +3400,11 @@
       <c r="F2" s="2" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>131</v>
       </c>
@@ -2891,8 +3417,11 @@
       <c r="F3" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="2" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>131</v>
       </c>
@@ -2905,8 +3434,11 @@
       <c r="F4" s="2" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="2" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>131</v>
       </c>
@@ -2919,8 +3451,11 @@
       <c r="F5" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G5" s="2" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>131</v>
       </c>
@@ -2933,8 +3468,11 @@
       <c r="F6" s="2" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G6" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2947,8 +3485,11 @@
       <c r="F7" s="2" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="G7" s="2" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -2961,8 +3502,11 @@
       <c r="F8" s="2" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="2" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -2975,8 +3519,11 @@
       <c r="F9" s="2" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="2" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -2989,8 +3536,11 @@
       <c r="F10" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G10" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -3003,8 +3553,11 @@
       <c r="F11" s="2" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G11" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -3017,8 +3570,11 @@
       <c r="F12" s="2" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G12" s="2" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -3031,8 +3587,11 @@
       <c r="F13" s="2" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G13" s="2" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -3045,8 +3604,11 @@
       <c r="F14" s="2" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -3059,8 +3621,11 @@
       <c r="F15" s="2" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -3073,8 +3638,11 @@
       <c r="F16" s="2" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>147</v>
       </c>
@@ -3084,8 +3652,11 @@
       <c r="F17" s="2" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>148</v>
       </c>
@@ -3095,8 +3666,11 @@
       <c r="F18" s="2" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>55</v>
       </c>
@@ -3106,8 +3680,11 @@
       <c r="F19" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>149</v>
       </c>
@@ -3117,8 +3694,11 @@
       <c r="F20" s="2" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>150</v>
       </c>
@@ -3128,8 +3708,11 @@
       <c r="F21" s="2" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="2" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>151</v>
       </c>
@@ -3139,8 +3722,11 @@
       <c r="F22" s="2" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G22" s="2" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>66</v>
       </c>
@@ -3150,8 +3736,11 @@
       <c r="F23" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G23" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>152</v>
       </c>
@@ -3161,8 +3750,11 @@
       <c r="F24" s="2" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G24" s="2" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>174</v>
       </c>
@@ -3175,8 +3767,11 @@
       <c r="F25" s="2" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" s="2" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>174</v>
       </c>
@@ -3189,8 +3784,11 @@
       <c r="F26" s="2" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" s="2" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>174</v>
       </c>
@@ -3203,8 +3801,11 @@
       <c r="F27" s="2" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G27" s="2" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>174</v>
       </c>
@@ -3217,8 +3818,11 @@
       <c r="F28" s="2" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G28" s="2" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>174</v>
       </c>
@@ -3231,8 +3835,11 @@
       <c r="F29" s="2" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G29" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>174</v>
       </c>
@@ -3245,8 +3852,11 @@
       <c r="F30" s="2" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G30" s="2" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>174</v>
       </c>
@@ -3259,8 +3869,11 @@
       <c r="F31" s="2" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G31" s="2" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>174</v>
       </c>
@@ -3273,8 +3886,11 @@
       <c r="F32" s="2" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G32" s="2" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>174</v>
       </c>
@@ -3287,8 +3903,11 @@
       <c r="F33" s="2" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G33" s="2" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>174</v>
       </c>
@@ -3301,8 +3920,11 @@
       <c r="F34" s="2" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G34" s="2" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>174</v>
       </c>
@@ -3315,8 +3937,11 @@
       <c r="F35" s="2" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G35" s="2" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>174</v>
       </c>
@@ -3329,8 +3954,11 @@
       <c r="F36" s="2" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G36" s="2" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>174</v>
       </c>
@@ -3343,8 +3971,11 @@
       <c r="F37" s="2" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G37" s="2" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>174</v>
       </c>
@@ -3357,8 +3988,11 @@
       <c r="F38" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G38" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>174</v>
       </c>
@@ -3371,8 +4005,11 @@
       <c r="F39" s="2" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G39" s="2" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>133</v>
       </c>
@@ -3388,8 +4025,11 @@
       <c r="F40" s="2" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G40" s="2" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>133</v>
       </c>
@@ -3405,8 +4045,11 @@
       <c r="F41" s="2" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G41" s="2" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>133</v>
       </c>
@@ -3422,8 +4065,11 @@
       <c r="F42" s="2" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G42" s="2" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>133</v>
       </c>
@@ -3436,8 +4082,11 @@
       <c r="F43" s="2" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G43" s="2" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>133</v>
       </c>
@@ -3450,8 +4099,11 @@
       <c r="F44" s="2" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G44" s="2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>133</v>
       </c>
@@ -3464,8 +4116,11 @@
       <c r="F45" s="2" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G45" s="2" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>133</v>
       </c>
@@ -3478,8 +4133,11 @@
       <c r="F46" s="2" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G46" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>133</v>
       </c>
@@ -3492,8 +4150,11 @@
       <c r="F47" s="2" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G47" s="2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>133</v>
       </c>
@@ -3506,8 +4167,11 @@
       <c r="F48" s="2" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G48" s="2" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>133</v>
       </c>
@@ -3520,8 +4184,11 @@
       <c r="F49" s="2" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G49" s="2" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>133</v>
       </c>
@@ -3534,8 +4201,11 @@
       <c r="F50" s="2" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G50" s="2" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>133</v>
       </c>
@@ -3548,8 +4218,11 @@
       <c r="F51" s="2" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G51" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>133</v>
       </c>
@@ -3562,8 +4235,11 @@
       <c r="F52" s="2" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G52" s="2" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>133</v>
       </c>
@@ -3576,8 +4252,11 @@
       <c r="F53" s="2" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" s="2" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>133</v>
       </c>
@@ -3590,8 +4269,11 @@
       <c r="F54" s="2" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G54" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>133</v>
       </c>
@@ -3604,8 +4286,11 @@
       <c r="F55" s="2" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G55" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>133</v>
       </c>
@@ -3618,8 +4303,11 @@
       <c r="F56" s="2" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G56" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>133</v>
       </c>
@@ -3632,8 +4320,11 @@
       <c r="F57" s="2" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57" s="2" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>133</v>
       </c>
@@ -3646,8 +4337,11 @@
       <c r="F58" s="2" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G58" s="2" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>133</v>
       </c>
@@ -3660,8 +4354,11 @@
       <c r="F59" s="2" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G59" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>133</v>
       </c>
@@ -3674,8 +4371,11 @@
       <c r="F60" s="2" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G60" s="2" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>134</v>
       </c>
@@ -3688,8 +4388,11 @@
       <c r="F61" s="2" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G61" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>134</v>
       </c>
@@ -3702,8 +4405,11 @@
       <c r="F62" s="2" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G62" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>134</v>
       </c>
@@ -3716,8 +4422,11 @@
       <c r="F63" s="2" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63" s="2" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>134</v>
       </c>
@@ -3730,8 +4439,11 @@
       <c r="F64" s="2" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G64" s="2" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>134</v>
       </c>
@@ -3744,1086 +4456,1284 @@
       <c r="F65" s="2" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G65" s="2" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>251</v>
+        <v>678</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>266</v>
+        <v>679</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+        <v>680</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>55</v>
+        <v>251</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>60</v>
+        <v>266</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+        <v>456</v>
+      </c>
+      <c r="G67" s="2" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>116</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>253</v>
+        <v>66</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>313</v>
+        <v>68</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>272</v>
+        <v>313</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+        <v>457</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+        <v>458</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+        <v>459</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+        <v>460</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+        <v>461</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>462</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+        <v>463</v>
+      </c>
+      <c r="G76" s="2" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+        <v>464</v>
+      </c>
+      <c r="G77" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+        <v>465</v>
+      </c>
+      <c r="G78" s="2" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+        <v>466</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+        <v>467</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>134</v>
       </c>
       <c r="B81" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="E82" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A82" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G82" s="2" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>285</v>
+        <v>682</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>315</v>
+        <v>686</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>147</v>
+        <v>303</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>156</v>
+        <v>333</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>316</v>
+        <v>689</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>317</v>
+        <v>690</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>288</v>
+        <v>683</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>318</v>
+        <v>691</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>289</v>
+        <v>684</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>319</v>
+        <v>695</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>290</v>
+        <v>685</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>320</v>
+        <v>696</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>252</v>
+        <v>314</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+        <v>469</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+        <v>470</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>322</v>
+        <v>156</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+        <v>413</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+        <v>471</v>
+      </c>
+      <c r="G93" s="2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+        <v>472</v>
+      </c>
+      <c r="G94" s="2" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+        <v>473</v>
+      </c>
+      <c r="G95" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>474</v>
+      </c>
+      <c r="G96" s="2" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+        <v>475</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>328</v>
+        <v>252</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+        <v>476</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>300</v>
+        <v>135</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+        <v>322</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>477</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+        <v>478</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+        <v>479</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+        <v>480</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>281</v>
+        <v>327</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>481</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>482</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>483</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>484</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>485</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>486</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>487</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B112" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>490</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>339</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>494</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B119" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B120" s="4" t="s">
         <v>312</v>
       </c>
-      <c r="E112" s="2" t="s">
+      <c r="E120" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="F112" s="2" t="s">
+      <c r="F120" s="2" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" s="4" t="s">
+      <c r="G120" s="2" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B113" s="4" t="s">
+      <c r="B121" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="E113" s="2" t="s">
+      <c r="E121" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F113" s="2" t="s">
+      <c r="F121" s="2" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" s="4" t="s">
+      <c r="G121" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B114" s="4" t="s">
+      <c r="B122" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E114" s="2" t="s">
+      <c r="E122" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="F122" s="2" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" s="4" t="s">
+      <c r="G122" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B115" s="4" t="s">
+      <c r="B123" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="E115" s="2" t="s">
+      <c r="E123" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="F115" s="2" t="s">
+      <c r="F123" s="2" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A116" s="4" t="s">
+      <c r="G123" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B116" s="4" t="s">
+      <c r="B124" s="4" t="s">
         <v>343</v>
       </c>
-      <c r="E116" s="2" t="s">
+      <c r="E124" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="F116" s="2" t="s">
+      <c r="F124" s="2" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A117" s="4" t="s">
+      <c r="G124" s="2" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B117" s="4" t="s">
+      <c r="B125" s="4" t="s">
         <v>344</v>
       </c>
-      <c r="E117" s="2" t="s">
+      <c r="E125" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="F117" s="2" t="s">
+      <c r="F125" s="2" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A118" s="4" t="s">
+      <c r="G125" s="2" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B118" s="4" t="s">
+      <c r="B126" s="4" t="s">
         <v>345</v>
       </c>
-      <c r="E118" s="2" t="s">
+      <c r="E126" s="2" t="s">
         <v>351</v>
       </c>
-      <c r="F118" s="2" t="s">
+      <c r="F126" s="2" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A119" s="4" t="s">
+      <c r="G126" s="2" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B119" s="4" t="s">
+      <c r="B127" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="E119" s="2" t="s">
+      <c r="E127" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="F127" s="2" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A120" s="4" t="s">
+      <c r="G127" s="2" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="s">
         <v>342</v>
       </c>
-      <c r="B120" s="4" t="s">
+      <c r="B128" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="E120" s="2" t="s">
+      <c r="E128" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F120" s="2" t="s">
+      <c r="F128" s="2" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A121" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B121" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A122" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B122" s="4" t="s">
-        <v>355</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A123" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B123" s="4" t="s">
-        <v>356</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A124" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B124" s="4" t="s">
-        <v>357</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A125" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B125" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="C125" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A126" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B126" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="C126" s="4" t="s">
-        <v>360</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A127" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B127" s="4" t="s">
-        <v>358</v>
-      </c>
-      <c r="C127" s="4" t="s">
-        <v>361</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="A128" s="4" t="s">
-        <v>354</v>
-      </c>
-      <c r="B128" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C128" s="4" t="s">
-        <v>362</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G128" s="2" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C129" s="4" t="s">
-        <v>291</v>
+        <v>698</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+        <v>699</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C130" s="4" t="s">
-        <v>355</v>
+        <v>291</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+        <v>375</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>388</v>
+        <v>355</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>376</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C132" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>377</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+        <v>378</v>
+      </c>
+      <c r="G133" s="2" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C134" s="4" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>379</v>
+      </c>
+      <c r="G134" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C135" s="4" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>380</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+        <v>381</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>364</v>
+        <v>35</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>382</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>364</v>
+        <v>35</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>357</v>
+        <v>291</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+        <v>383</v>
+      </c>
+      <c r="G138" s="2" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>364</v>
+        <v>35</v>
       </c>
       <c r="C139" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D139" s="4" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>384</v>
+      </c>
+      <c r="G139" s="2" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>364</v>
+        <v>35</v>
       </c>
       <c r="C140" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D140" s="4" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>385</v>
+      </c>
+      <c r="G140" s="2" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>364</v>
+        <v>35</v>
       </c>
       <c r="C141" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D141" s="4" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>386</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B142" s="4" t="s">
-        <v>364</v>
+        <v>35</v>
       </c>
       <c r="C142" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D142" s="4" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
         <v>354</v>
       </c>
@@ -4831,16 +5741,16 @@
         <v>364</v>
       </c>
       <c r="C143" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D143" s="4" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>389</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>354</v>
       </c>
@@ -4848,55 +5758,235 @@
         <v>364</v>
       </c>
       <c r="C144" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="D144" s="4" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>390</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
         <v>354</v>
       </c>
       <c r="B145" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="G145" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A146" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="E146" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="G146" s="2" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="E147" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E148" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="G148" s="2" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A149" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A150" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B150" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D150" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A151" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B151" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D151" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="E151" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="G151" s="2" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A152" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E152" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="G152" s="2" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A153" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>399</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A154" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B154" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C145" s="4" t="s">
+      <c r="C154" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="E145" s="2" t="s">
+      <c r="E154" s="2" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A146" s="4" t="s">
+      <c r="G154" s="2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A155" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="B146" s="4" t="s">
+      <c r="B155" s="4" t="s">
         <v>291</v>
       </c>
-      <c r="E146" s="2" t="s">
+      <c r="E155" s="2" t="s">
         <v>401</v>
       </c>
-      <c r="F146" s="2" t="s">
+      <c r="F155" s="2" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A147" s="4" t="s">
+      <c r="G155" s="2" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A156" s="4" t="s">
         <v>374</v>
       </c>
-      <c r="B147" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="E147" s="2" t="s">
+      <c r="E156" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="F147" s="2" t="s">
+      <c r="F156" s="2" t="s">
         <v>503</v>
+      </c>
+      <c r="G156" s="2" t="s">
+        <v>669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added german translations, new helper methods, new build
</commit_message>
<xml_diff>
--- a/docs/CMDI Maker Localisations.xlsx
+++ b/docs/CMDI Maker Localisations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="588"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="588" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="APP CORE" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="726">
   <si>
     <t>Key1</t>
   </si>
@@ -2140,6 +2140,81 @@
   </si>
   <si>
     <t>ZIP-Archiv herunterladen</t>
+  </si>
+  <si>
+    <t>Ein kurzer Name oder eine Abkürzung bestehend aus einem oder zwei Wörtern. Diese Kennung unterscheidet die Session von anderen im selben Korpus und wird beim schnellen Browsen genutzt.</t>
+  </si>
+  <si>
+    <t>Der "Session Title" ist der komplette Titel der Session ohne Abkürzungen.</t>
+  </si>
+  <si>
+    <t>Im Allgemeinen ist das primäre Datum der Session das Datum der Aufzeichnungen. Wenn diese Session Written Resources enthält, steht hier das Erstellungsdatum des primären Dokumentes.</t>
+  </si>
+  <si>
+    <t>Hier kann eine Beschreibung eingegeben werden, die die Session als Ganzes beschreibt: Beispiel: Eine Unterhaltung zwischen Mutter, Vater und Kind am Frühstückstisch.</t>
+  </si>
+  <si>
+    <t>Wenn es im Dokument um die "Sprachen von Südamerika" geht, sollte nur der Kontinent genannt werden.</t>
+  </si>
+  <si>
+    <t>Dieses Element kann auch genutzt werden, um Sub-Regionen zu beschreiben. Beispiele: Europa, die Niederlande, Achterhoek.</t>
+  </si>
+  <si>
+    <t>Falls die Aufnahmen beispielsweise in einem Institut gemacht worden sind, sollte hier die Adresse des Instituts eingegeben werden.</t>
+  </si>
+  <si>
+    <t>Wenn die Session innerhalb eines Projektes erstellt worden ist, enthält das Element "Project" Informationen über das Projekt. Diese Informationen werden typischerweise für viele Sessions wiederverwendet, wenn diese alle zum gleichen Projekt gehören.</t>
+  </si>
+  <si>
+    <t>Ein kurzer Name oder eine Abkürzung des Projektes.</t>
+  </si>
+  <si>
+    <t>Der komplette und ausführliche Titel des Projektes.</t>
+  </si>
+  <si>
+    <t>Eine eindeutige Kennung für das Projekt.</t>
+  </si>
+  <si>
+    <t>Eine ausführliche Beschreibung über den Umfang des Projektes und über seine Ziele.</t>
+  </si>
+  <si>
+    <t>Kontaktinformationen der Person oder der Institution, die für das Projekt verantwortlich ist.</t>
+  </si>
+  <si>
+    <t>Die "Content"-Spalte wird benutzt, um den Inhalt der Sessions zu beschreiben. Dies geschieht mit Hilfe der 4 Dimensionen "Communication Context", "Genre", "Task" und "Modalities".</t>
+  </si>
+  <si>
+    <t>Der konventionalisierte Typ des Inhalts der Session.</t>
+  </si>
+  <si>
+    <t>Der konventionalisierte Sub-Typ des Inhalts der Session.</t>
+  </si>
+  <si>
+    <t>In Bereichen wie der Sprachdatenverarbeitung geht es oftmals um typische Aufgaben oder Situationen wie "info kiosk task" oder "frog story".</t>
+  </si>
+  <si>
+    <t>Im Gegensatz zu den anderen Elementen, kann hier Volltext benutzt werden, um den Inhalt zu beschreiben.</t>
+  </si>
+  <si>
+    <t>Diese Gruppe von Elementen wird benutzt, um den Kontext der Kommunikation zu beschreiben, in dem die Aufnahme stattgefunden hat.</t>
+  </si>
+  <si>
+    <t>Struktur des Kontextes der Kommunikation.</t>
+  </si>
+  <si>
+    <t>Weist darauf hin, in wie weit der Referent das linguistische Ereignis geplant hat.</t>
+  </si>
+  <si>
+    <t>Beschreibt den Grad der Interaktivität zwischen allen Actors in der Session.</t>
+  </si>
+  <si>
+    <t>Beschreibt den sozialen Kontext, in dem das Ereignis stattgefunden hat.</t>
+  </si>
+  <si>
+    <t>Beschreibt, in wie weit der Forscher in das Ereignis involviert war.</t>
+  </si>
+  <si>
+    <t>Diese Beschreibung betrifft alle Actors und sollte genutzt werden, um die Interaktionen und Beziehungen zwischen den Actors zu beschreiben.</t>
   </si>
 </sst>
 </file>
@@ -2177,7 +2252,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2199,6 +2274,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2230,7 +2311,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2244,6 +2325,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2528,8 +2612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
@@ -3346,9 +3430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G156"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G129" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4762,6 +4846,7 @@
       <c r="F83" s="2" t="s">
         <v>687</v>
       </c>
+      <c r="G83" s="7"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
@@ -4776,6 +4861,7 @@
       <c r="F84" s="2" t="s">
         <v>487</v>
       </c>
+      <c r="G84" s="7"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
@@ -4790,6 +4876,7 @@
       <c r="F85" s="2" t="s">
         <v>488</v>
       </c>
+      <c r="G85" s="7"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
@@ -4804,8 +4891,9 @@
       <c r="F86" s="2" t="s">
         <v>688</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G86" s="7"/>
+    </row>
+    <row r="87" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>134</v>
       </c>
@@ -4818,6 +4906,7 @@
       <c r="F87" s="2" t="s">
         <v>692</v>
       </c>
+      <c r="G87" s="7"/>
     </row>
     <row r="88" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
@@ -4832,6 +4921,7 @@
       <c r="F88" s="2" t="s">
         <v>693</v>
       </c>
+      <c r="G88" s="7"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
@@ -4846,6 +4936,7 @@
       <c r="F89" s="2" t="s">
         <v>694</v>
       </c>
+      <c r="G89" s="7"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
@@ -5523,6 +5614,7 @@
       <c r="F129" s="2" t="s">
         <v>700</v>
       </c>
+      <c r="G129" s="7"/>
     </row>
     <row r="130" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
@@ -5534,6 +5626,9 @@
       <c r="E130" s="2" t="s">
         <v>375</v>
       </c>
+      <c r="F130" s="2" t="s">
+        <v>701</v>
+      </c>
       <c r="G130" s="2" t="s">
         <v>643</v>
       </c>
@@ -5548,6 +5643,9 @@
       <c r="E131" s="2" t="s">
         <v>376</v>
       </c>
+      <c r="F131" s="2" t="s">
+        <v>702</v>
+      </c>
       <c r="G131" s="2" t="s">
         <v>644</v>
       </c>
@@ -5562,6 +5660,9 @@
       <c r="E132" s="2" t="s">
         <v>377</v>
       </c>
+      <c r="F132" s="2" t="s">
+        <v>703</v>
+      </c>
       <c r="G132" s="2" t="s">
         <v>645</v>
       </c>
@@ -5576,6 +5677,9 @@
       <c r="E133" s="2" t="s">
         <v>378</v>
       </c>
+      <c r="F133" s="2" t="s">
+        <v>704</v>
+      </c>
       <c r="G133" s="2" t="s">
         <v>646</v>
       </c>
@@ -5593,6 +5697,9 @@
       <c r="E134" s="2" t="s">
         <v>379</v>
       </c>
+      <c r="F134" s="2" t="s">
+        <v>705</v>
+      </c>
       <c r="G134" s="2" t="s">
         <v>647</v>
       </c>
@@ -5610,6 +5717,9 @@
       <c r="E135" s="2" t="s">
         <v>380</v>
       </c>
+      <c r="F135" s="2" t="s">
+        <v>706</v>
+      </c>
       <c r="G135" s="2" t="s">
         <v>648</v>
       </c>
@@ -5627,6 +5737,9 @@
       <c r="E136" s="2" t="s">
         <v>381</v>
       </c>
+      <c r="F136" s="2" t="s">
+        <v>707</v>
+      </c>
       <c r="G136" s="2" t="s">
         <v>649</v>
       </c>
@@ -5644,6 +5757,9 @@
       <c r="E137" s="2" t="s">
         <v>382</v>
       </c>
+      <c r="F137" s="2" t="s">
+        <v>708</v>
+      </c>
       <c r="G137" s="2" t="s">
         <v>650</v>
       </c>
@@ -5661,11 +5777,14 @@
       <c r="E138" s="2" t="s">
         <v>383</v>
       </c>
+      <c r="F138" s="2" t="s">
+        <v>709</v>
+      </c>
       <c r="G138" s="2" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
         <v>354</v>
       </c>
@@ -5677,6 +5796,9 @@
       </c>
       <c r="E139" s="2" t="s">
         <v>384</v>
+      </c>
+      <c r="F139" s="2" t="s">
+        <v>710</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>652</v>
@@ -5695,6 +5817,9 @@
       <c r="E140" s="2" t="s">
         <v>385</v>
       </c>
+      <c r="F140" s="2" t="s">
+        <v>711</v>
+      </c>
       <c r="G140" s="2" t="s">
         <v>653</v>
       </c>
@@ -5712,6 +5837,9 @@
       <c r="E141" s="2" t="s">
         <v>386</v>
       </c>
+      <c r="F141" s="2" t="s">
+        <v>712</v>
+      </c>
       <c r="G141" s="2" t="s">
         <v>654</v>
       </c>
@@ -5729,6 +5857,9 @@
       <c r="E142" s="2" t="s">
         <v>387</v>
       </c>
+      <c r="F142" s="2" t="s">
+        <v>713</v>
+      </c>
       <c r="G142" s="2" t="s">
         <v>655</v>
       </c>
@@ -5746,6 +5877,9 @@
       <c r="E143" s="2" t="s">
         <v>389</v>
       </c>
+      <c r="F143" s="2" t="s">
+        <v>714</v>
+      </c>
       <c r="G143" s="2" t="s">
         <v>656</v>
       </c>
@@ -5763,6 +5897,9 @@
       <c r="E144" s="2" t="s">
         <v>390</v>
       </c>
+      <c r="F144" s="2" t="s">
+        <v>715</v>
+      </c>
       <c r="G144" s="2" t="s">
         <v>657</v>
       </c>
@@ -5780,6 +5917,9 @@
       <c r="E145" s="2" t="s">
         <v>391</v>
       </c>
+      <c r="F145" s="2" t="s">
+        <v>716</v>
+      </c>
       <c r="G145" s="2" t="s">
         <v>658</v>
       </c>
@@ -5797,11 +5937,14 @@
       <c r="E146" s="2" t="s">
         <v>392</v>
       </c>
+      <c r="F146" s="2" t="s">
+        <v>717</v>
+      </c>
       <c r="G146" s="2" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
         <v>354</v>
       </c>
@@ -5814,11 +5957,14 @@
       <c r="E147" s="2" t="s">
         <v>393</v>
       </c>
+      <c r="F147" s="2" t="s">
+        <v>718</v>
+      </c>
       <c r="G147" s="2" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
         <v>354</v>
       </c>
@@ -5833,6 +5979,9 @@
       </c>
       <c r="E148" s="2" t="s">
         <v>394</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>719</v>
       </c>
       <c r="G148" s="2" t="s">
         <v>661</v>
@@ -5854,11 +6003,14 @@
       <c r="E149" s="2" t="s">
         <v>395</v>
       </c>
+      <c r="F149" s="2" t="s">
+        <v>720</v>
+      </c>
       <c r="G149" s="2" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
         <v>354</v>
       </c>
@@ -5873,6 +6025,9 @@
       </c>
       <c r="E150" s="2" t="s">
         <v>396</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>721</v>
       </c>
       <c r="G150" s="2" t="s">
         <v>663</v>
@@ -5894,6 +6049,9 @@
       <c r="E151" s="2" t="s">
         <v>397</v>
       </c>
+      <c r="F151" s="2" t="s">
+        <v>722</v>
+      </c>
       <c r="G151" s="2" t="s">
         <v>664</v>
       </c>
@@ -5914,6 +6072,9 @@
       <c r="E152" s="2" t="s">
         <v>398</v>
       </c>
+      <c r="F152" s="2" t="s">
+        <v>723</v>
+      </c>
       <c r="G152" s="2" t="s">
         <v>665</v>
       </c>
@@ -5934,6 +6095,9 @@
       <c r="E153" s="2" t="s">
         <v>399</v>
       </c>
+      <c r="F153" s="2" t="s">
+        <v>724</v>
+      </c>
       <c r="G153" s="2" t="s">
         <v>666</v>
       </c>
@@ -5950,6 +6114,9 @@
       </c>
       <c r="E154" s="2" t="s">
         <v>400</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>725</v>
       </c>
       <c r="G154" s="2" t="s">
         <v>667</v>

</xml_diff>

<commit_message>
Code smoothing, new IMDI tutorial in Help Pages
</commit_message>
<xml_diff>
--- a/docs/CMDI Maker Localisations.xlsx
+++ b/docs/CMDI Maker Localisations.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="1170"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="1176"/>
   </bookViews>
   <sheets>
     <sheet name="APP CORE" sheetId="1" r:id="rId1"/>
     <sheet name="IMDI Environment" sheetId="3" r:id="rId2"/>
     <sheet name="ELDP Environment" sheetId="4" r:id="rId3"/>
+    <sheet name="Advice" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="748">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1062" uniqueCount="750">
   <si>
     <t>Key1</t>
   </si>
@@ -2059,12 +2060,6 @@
     <t>Exportar a archivo</t>
   </si>
   <si>
-    <t>In Datei exportieren</t>
-  </si>
-  <si>
-    <t>Export to file</t>
-  </si>
-  <si>
     <t>Este archivo multimedia no es un archivo  de recursos válido para LAMUS. Por favor intente convertir su código en formato WAV (audio) o en MP4 (video).</t>
   </si>
   <si>
@@ -2251,12 +2246,6 @@
     <t>Abbrechen</t>
   </si>
   <si>
-    <t>Open File</t>
-  </si>
-  <si>
-    <t>Datei öffnen</t>
-  </si>
-  <si>
     <t>Anular</t>
   </si>
   <si>
@@ -2282,6 +2271,24 @@
   </si>
   <si>
     <t>Es gibt keine Daten zum Speichern, da kein Profil geladen ist.</t>
+  </si>
+  <si>
+    <t>If not sure about translating tech terms, maybe Microsoft Terminology Search is of help</t>
+  </si>
+  <si>
+    <t>http://www.microsoft.com/Language/en-US/Search.aspx?sString=Abort&amp;langID=es-es</t>
+  </si>
+  <si>
+    <t>Export Project to file</t>
+  </si>
+  <si>
+    <t>Open Project File</t>
+  </si>
+  <si>
+    <t>Projekt in Datei exportieren</t>
+  </si>
+  <si>
+    <t>Projektdatei öffnen</t>
   </si>
 </sst>
 </file>
@@ -2671,24 +2678,24 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="4"/>
+    <col min="1" max="1" width="11.44140625" style="4"/>
     <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="4"/>
+    <col min="3" max="3" width="15.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="4"/>
     <col min="5" max="5" width="31" style="2" customWidth="1"/>
     <col min="6" max="6" width="32" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
+    <col min="7" max="7" width="31.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2711,7 +2718,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
@@ -2728,7 +2735,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -2745,7 +2752,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2762,7 +2769,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
@@ -2779,7 +2786,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -2796,7 +2803,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -2813,7 +2820,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -2830,7 +2837,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -2847,7 +2854,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -2864,7 +2871,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -2881,7 +2888,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -2898,7 +2905,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -2915,7 +2922,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -2932,7 +2939,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -2949,7 +2956,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -2966,7 +2973,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -2983,7 +2990,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -3000,7 +3007,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
@@ -3017,7 +3024,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
@@ -3034,7 +3041,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -3051,7 +3058,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -3068,7 +3075,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>50</v>
       </c>
@@ -3085,7 +3092,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>50</v>
       </c>
@@ -3102,12 +3109,12 @@
         <v>506</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>53</v>
@@ -3119,21 +3126,21 @@
         <v>507</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>747</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
@@ -3150,7 +3157,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
@@ -3167,7 +3174,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>54</v>
       </c>
@@ -3184,7 +3191,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>54</v>
       </c>
@@ -3201,7 +3208,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>54</v>
       </c>
@@ -3218,7 +3225,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>65</v>
       </c>
@@ -3232,7 +3239,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>11</v>
       </c>
@@ -3246,7 +3253,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>66</v>
       </c>
@@ -3260,7 +3267,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>69</v>
       </c>
@@ -3274,7 +3281,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>71</v>
       </c>
@@ -3288,7 +3295,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>72</v>
       </c>
@@ -3302,49 +3309,49 @@
         <v>516</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>671</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>674</v>
+        <v>746</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>673</v>
+        <v>748</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>672</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>733</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>737</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>738</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="F40" s="2" t="s">
         <v>734</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="F40" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>739</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>75</v>
       </c>
@@ -3361,7 +3368,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>75</v>
       </c>
@@ -3378,7 +3385,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>75</v>
       </c>
@@ -3395,7 +3402,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>75</v>
       </c>
@@ -3412,7 +3419,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>75</v>
       </c>
@@ -3429,7 +3436,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>75</v>
       </c>
@@ -3446,7 +3453,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>75</v>
       </c>
@@ -3466,7 +3473,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>75</v>
       </c>
@@ -3486,7 +3493,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>176</v>
       </c>
@@ -3503,7 +3510,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>176</v>
       </c>
@@ -3535,20 +3542,20 @@
       <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="4"/>
+    <col min="1" max="1" width="11.44140625" style="4"/>
     <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="4"/>
-    <col min="5" max="5" width="30.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="4"/>
+    <col min="5" max="5" width="30.44140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="32" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
+    <col min="7" max="7" width="31.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3571,7 +3578,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>130</v>
       </c>
@@ -3588,7 +3595,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>130</v>
       </c>
@@ -3605,7 +3612,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>130</v>
       </c>
@@ -3622,7 +3629,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>130</v>
       </c>
@@ -3639,7 +3646,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>130</v>
       </c>
@@ -3656,7 +3663,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -3673,7 +3680,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -3690,7 +3697,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
@@ -3707,7 +3714,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -3724,7 +3731,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>4</v>
       </c>
@@ -3741,7 +3748,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>4</v>
       </c>
@@ -3758,7 +3765,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
@@ -3775,7 +3782,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>4</v>
       </c>
@@ -3792,7 +3799,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>4</v>
       </c>
@@ -3809,7 +3816,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>4</v>
       </c>
@@ -3826,7 +3833,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>146</v>
       </c>
@@ -3840,7 +3847,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>147</v>
       </c>
@@ -3854,7 +3861,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>55</v>
       </c>
@@ -3868,7 +3875,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>148</v>
       </c>
@@ -3882,7 +3889,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>149</v>
       </c>
@@ -3896,7 +3903,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>150</v>
       </c>
@@ -3910,7 +3917,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>66</v>
       </c>
@@ -3924,7 +3931,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>151</v>
       </c>
@@ -3938,7 +3945,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>173</v>
       </c>
@@ -3955,7 +3962,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>173</v>
       </c>
@@ -3972,7 +3979,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>173</v>
       </c>
@@ -3989,7 +3996,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>173</v>
       </c>
@@ -4006,7 +4013,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>173</v>
       </c>
@@ -4023,7 +4030,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>173</v>
       </c>
@@ -4040,7 +4047,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>173</v>
       </c>
@@ -4057,7 +4064,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>173</v>
       </c>
@@ -4074,7 +4081,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>173</v>
       </c>
@@ -4091,7 +4098,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>173</v>
       </c>
@@ -4108,7 +4115,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>173</v>
       </c>
@@ -4125,7 +4132,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>173</v>
       </c>
@@ -4142,7 +4149,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>173</v>
       </c>
@@ -4159,7 +4166,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>173</v>
       </c>
@@ -4176,7 +4183,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>173</v>
       </c>
@@ -4193,7 +4200,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>132</v>
       </c>
@@ -4213,7 +4220,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>132</v>
       </c>
@@ -4230,10 +4237,10 @@
         <v>433</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>132</v>
       </c>
@@ -4250,10 +4257,10 @@
         <v>434</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>132</v>
       </c>
@@ -4270,7 +4277,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>132</v>
       </c>
@@ -4287,7 +4294,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>132</v>
       </c>
@@ -4304,7 +4311,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>132</v>
       </c>
@@ -4321,7 +4328,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>132</v>
       </c>
@@ -4338,7 +4345,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>132</v>
       </c>
@@ -4355,7 +4362,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>132</v>
       </c>
@@ -4372,7 +4379,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>132</v>
       </c>
@@ -4389,7 +4396,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>132</v>
       </c>
@@ -4406,7 +4413,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>132</v>
       </c>
@@ -4423,7 +4430,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>132</v>
       </c>
@@ -4440,7 +4447,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>132</v>
       </c>
@@ -4457,7 +4464,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>132</v>
       </c>
@@ -4474,7 +4481,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>132</v>
       </c>
@@ -4491,7 +4498,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>132</v>
       </c>
@@ -4508,7 +4515,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>132</v>
       </c>
@@ -4525,7 +4532,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>132</v>
       </c>
@@ -4542,7 +4549,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>132</v>
       </c>
@@ -4559,7 +4566,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>133</v>
       </c>
@@ -4576,7 +4583,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>133</v>
       </c>
@@ -4593,24 +4600,24 @@
         <v>592</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>410</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>133</v>
       </c>
@@ -4627,7 +4634,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>133</v>
       </c>
@@ -4644,7 +4651,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>133</v>
       </c>
@@ -4661,24 +4668,24 @@
         <v>595</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="F67" s="2" t="s">
         <v>677</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="G67" s="2" t="s">
         <v>678</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>679</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>133</v>
       </c>
@@ -4695,7 +4702,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>133</v>
       </c>
@@ -4712,7 +4719,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>133</v>
       </c>
@@ -4729,7 +4736,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>133</v>
       </c>
@@ -4746,7 +4753,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>133</v>
       </c>
@@ -4763,7 +4770,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>133</v>
       </c>
@@ -4780,7 +4787,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>133</v>
       </c>
@@ -4797,7 +4804,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>133</v>
       </c>
@@ -4814,7 +4821,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>133</v>
       </c>
@@ -4831,7 +4838,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>133</v>
       </c>
@@ -4848,7 +4855,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>133</v>
       </c>
@@ -4865,7 +4872,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>133</v>
       </c>
@@ -4882,7 +4889,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>133</v>
       </c>
@@ -4899,7 +4906,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>133</v>
       </c>
@@ -4916,7 +4923,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>133</v>
       </c>
@@ -4933,7 +4940,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>133</v>
       </c>
@@ -4950,24 +4957,24 @@
         <v>608</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>133</v>
       </c>
@@ -4981,10 +4988,10 @@
         <v>486</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>725</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>133</v>
       </c>
@@ -4992,16 +4999,16 @@
         <v>303</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F86" s="2" t="s">
         <v>487</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>133</v>
       </c>
@@ -5009,67 +5016,67 @@
         <v>304</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>729</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>133</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>134</v>
       </c>
@@ -5086,7 +5093,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>134</v>
       </c>
@@ -5103,7 +5110,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>134</v>
       </c>
@@ -5120,7 +5127,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>134</v>
       </c>
@@ -5137,7 +5144,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>134</v>
       </c>
@@ -5154,7 +5161,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>134</v>
       </c>
@@ -5171,7 +5178,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>134</v>
       </c>
@@ -5188,7 +5195,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>134</v>
       </c>
@@ -5205,7 +5212,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>134</v>
       </c>
@@ -5222,7 +5229,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>134</v>
       </c>
@@ -5239,7 +5246,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>134</v>
       </c>
@@ -5256,7 +5263,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>134</v>
       </c>
@@ -5273,7 +5280,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>134</v>
       </c>
@@ -5290,7 +5297,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>134</v>
       </c>
@@ -5307,7 +5314,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>134</v>
       </c>
@@ -5324,7 +5331,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>134</v>
       </c>
@@ -5341,7 +5348,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>134</v>
       </c>
@@ -5358,7 +5365,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>134</v>
       </c>
@@ -5375,7 +5382,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>134</v>
       </c>
@@ -5392,7 +5399,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>134</v>
       </c>
@@ -5409,7 +5416,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>134</v>
       </c>
@@ -5426,7 +5433,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>134</v>
       </c>
@@ -5440,10 +5447,10 @@
         <v>486</v>
       </c>
       <c r="G112" s="2" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>134</v>
       </c>
@@ -5460,7 +5467,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>134</v>
       </c>
@@ -5477,7 +5484,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>134</v>
       </c>
@@ -5494,7 +5501,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>134</v>
       </c>
@@ -5511,7 +5518,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117" s="4" t="s">
         <v>134</v>
       </c>
@@ -5528,7 +5535,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A118" s="4" t="s">
         <v>134</v>
       </c>
@@ -5545,7 +5552,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>134</v>
       </c>
@@ -5562,7 +5569,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>134</v>
       </c>
@@ -5579,7 +5586,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" s="4" t="s">
         <v>134</v>
       </c>
@@ -5596,7 +5603,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>341</v>
       </c>
@@ -5613,7 +5620,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>341</v>
       </c>
@@ -5630,7 +5637,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>341</v>
       </c>
@@ -5647,7 +5654,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
         <v>341</v>
       </c>
@@ -5664,7 +5671,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
         <v>341</v>
       </c>
@@ -5681,7 +5688,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
         <v>341</v>
       </c>
@@ -5698,7 +5705,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
         <v>341</v>
       </c>
@@ -5715,7 +5722,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
         <v>341</v>
       </c>
@@ -5732,24 +5739,24 @@
         <v>641</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>341</v>
       </c>
       <c r="B130" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>695</v>
+      </c>
+      <c r="F130" s="2" t="s">
         <v>696</v>
       </c>
-      <c r="E130" s="2" t="s">
-        <v>697</v>
-      </c>
-      <c r="F130" s="2" t="s">
-        <v>698</v>
-      </c>
       <c r="G130" s="6" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>353</v>
       </c>
@@ -5760,13 +5767,13 @@
         <v>374</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G131" s="2" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>353</v>
       </c>
@@ -5777,13 +5784,13 @@
         <v>375</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>353</v>
       </c>
@@ -5794,13 +5801,13 @@
         <v>376</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>353</v>
       </c>
@@ -5811,13 +5818,13 @@
         <v>377</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
         <v>353</v>
       </c>
@@ -5831,13 +5838,13 @@
         <v>378</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>353</v>
       </c>
@@ -5851,13 +5858,13 @@
         <v>379</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
         <v>353</v>
       </c>
@@ -5871,13 +5878,13 @@
         <v>380</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>353</v>
       </c>
@@ -5891,13 +5898,13 @@
         <v>381</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
         <v>353</v>
       </c>
@@ -5911,13 +5918,13 @@
         <v>382</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>650</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
         <v>353</v>
       </c>
@@ -5931,13 +5938,13 @@
         <v>383</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="G140" s="2" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
         <v>353</v>
       </c>
@@ -5951,13 +5958,13 @@
         <v>384</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="G141" s="2" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
         <v>353</v>
       </c>
@@ -5971,13 +5978,13 @@
         <v>385</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="G142" s="2" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
         <v>353</v>
       </c>
@@ -5991,13 +5998,13 @@
         <v>386</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="G143" s="2" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>353</v>
       </c>
@@ -6011,13 +6018,13 @@
         <v>388</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
         <v>353</v>
       </c>
@@ -6031,13 +6038,13 @@
         <v>389</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A146" s="4" t="s">
         <v>353</v>
       </c>
@@ -6051,13 +6058,13 @@
         <v>390</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
         <v>353</v>
       </c>
@@ -6071,13 +6078,13 @@
         <v>391</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
         <v>353</v>
       </c>
@@ -6091,13 +6098,13 @@
         <v>392</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="G148" s="2" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="72" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
         <v>353</v>
       </c>
@@ -6114,13 +6121,13 @@
         <v>393</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="G149" s="2" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
         <v>353</v>
       </c>
@@ -6137,13 +6144,13 @@
         <v>394</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="G150" s="2" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
         <v>353</v>
       </c>
@@ -6160,13 +6167,13 @@
         <v>395</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="G151" s="2" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
         <v>353</v>
       </c>
@@ -6183,13 +6190,13 @@
         <v>396</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="G152" s="2" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
         <v>353</v>
       </c>
@@ -6206,13 +6213,13 @@
         <v>397</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="G153" s="2" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
         <v>353</v>
       </c>
@@ -6229,13 +6236,13 @@
         <v>398</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="G154" s="2" t="s">
         <v>665</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
         <v>353</v>
       </c>
@@ -6249,13 +6256,13 @@
         <v>399</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="G155" s="2" t="s">
         <v>666</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" s="4" t="s">
         <v>373</v>
       </c>
@@ -6272,7 +6279,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" s="4" t="s">
         <v>373</v>
       </c>
@@ -6304,20 +6311,20 @@
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="4"/>
+    <col min="1" max="1" width="11.44140625" style="4"/>
     <col min="2" max="2" width="21" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="4"/>
-    <col min="5" max="5" width="30.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="4"/>
+    <col min="5" max="5" width="30.44140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="32" style="2" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="26.7109375" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
+    <col min="7" max="7" width="31.33203125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="51.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6340,32 +6347,57 @@
         <v>540</v>
       </c>
     </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G83" s="6"/>
     </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G84" s="6"/>
     </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G85" s="6"/>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G86" s="6"/>
     </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G87" s="6"/>
     </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G88" s="6"/>
     </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G89" s="6"/>
     </row>
-    <row r="129" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G129" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>745</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>